<commit_message>
Completed Data Driven approach
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/customerData.xlsx
+++ b/src/test/resources/testData/customerData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="45">
   <si>
     <t>Make</t>
   </si>
@@ -505,8 +505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="Z2" sqref="Z2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -622,11 +622,11 @@
       <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="C2">
-        <v>600</v>
-      </c>
-      <c r="D2">
-        <v>600</v>
+      <c r="C2" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>39</v>
       </c>
       <c r="E2" s="2">
         <v>45352</v>

</xml_diff>